<commit_message>
Finishing of RP assignment 5
</commit_message>
<xml_diff>
--- a/period-2/pattern-recognition/tarea05/reporte/analisis-resultados.xlsx
+++ b/period-2/pattern-recognition/tarea05/reporte/analisis-resultados.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinvestav\github\Phd-Courses\period-2\pattern-recognition\tarea05\reporte\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
   </bookViews>
@@ -19,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>dataset</t>
   </si>
   <si>
-    <t>tiempo estimado ejecucion total</t>
-  </si>
-  <si>
     <t>tiempo promedio por configuración</t>
   </si>
   <si>
@@ -52,6 +54,15 @@
   </si>
   <si>
     <t>error promedio</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>nu</t>
   </si>
 </sst>
 </file>
@@ -112,9 +123,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -123,6 +136,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -448,32 +469,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A5" sqref="A5:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>73229.786059999999</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -484,66 +505,108 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C6">
+        <v>8.9108999999999994E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.3644</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>25528</v>
-      </c>
-      <c r="C6">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.3644</v>
+      <c r="B7">
+        <v>12.9</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.19670000000000001</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="G7">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>19276</v>
-      </c>
-      <c r="C7">
+      <c r="B8">
         <v>12.9</v>
       </c>
-      <c r="E7">
-        <v>0.19670000000000001</v>
+      <c r="C8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D8">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="G8">
+        <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>19200</v>
-      </c>
-      <c r="C8">
-        <v>12.9</v>
-      </c>
-      <c r="E8">
-        <v>0.12609999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
       <c r="B9">
-        <v>9224</v>
+        <v>6.1</v>
       </c>
       <c r="C9">
-        <v>6.1</v>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>4.5900000000000003E-2</v>
       </c>
       <c r="E9">
-        <v>4.5900000000000003E-2</v>
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="G9">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>